<commit_message>
Opschonen theVault: JavaDoc, Review document, dode code
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint 3/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint 3/ReviewDoc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carme\Documents\Vijf opleidingsonderdelen\Web App\the_Vault\src\main\resources\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48EB4601-9700-4071-AC5A-823C823A51A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67395EC-8EC2-4117-933D-A062C668BE2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="46">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -146,6 +146,24 @@
   </si>
   <si>
     <t>TransactieController</t>
+  </si>
+  <si>
+    <t>TransactiePaginaDto</t>
+  </si>
+  <si>
+    <t>TransactieStartDto</t>
+  </si>
+  <si>
+    <t>TransactieService</t>
+  </si>
+  <si>
+    <t>Carmen en</t>
+  </si>
+  <si>
+    <t>AssetDto</t>
+  </si>
+  <si>
+    <t>AssetNotExistsException</t>
   </si>
 </sst>
 </file>
@@ -538,8 +556,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <pane ySplit="7" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +605,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -873,36 +891,56 @@
       <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
+      <c r="A30" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+      <c r="A31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
+      <c r="A32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
+      <c r="A33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="7"/>

</xml_diff>